<commit_message>
Atualiza datasets das ligas
</commit_message>
<xml_diff>
--- a/liga_classica/datasets_liga_classica/Pontuacoes_Liga_Classica_Aluna_Completa.xlsx
+++ b/liga_classica/datasets_liga_classica/Pontuacoes_Liga_Classica_Aluna_Completa.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="56">
   <si>
     <t>Rodada 1</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>NHU PORÃ SAF.</t>
+  </si>
+  <si>
+    <t>Pepe Leal FC</t>
   </si>
   <si>
     <t>Pontaç0 F.C.</t>
@@ -544,7 +547,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM18"/>
+  <dimension ref="A1:AM19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2689,6 +2692,125 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="1:39">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
+        <v>0</v>
+      </c>
+      <c r="AH19">
+        <v>0</v>
+      </c>
+      <c r="AI19">
+        <v>0</v>
+      </c>
+      <c r="AJ19">
+        <v>0</v>
+      </c>
+      <c r="AK19">
+        <v>0</v>
+      </c>
+      <c r="AL19">
+        <v>0</v>
+      </c>
+      <c r="AM19">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2696,7 +2818,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3815,6 +3937,68 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3822,7 +4006,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3843,7 +4027,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3851,7 +4035,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -3859,7 +4043,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3867,7 +4051,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3875,7 +4059,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3883,7 +4067,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3891,7 +4075,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -3899,7 +4083,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3907,7 +4091,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3915,7 +4099,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3923,7 +4107,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -3931,7 +4115,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -3939,7 +4123,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -3947,7 +4131,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -3955,7 +4139,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -3963,9 +4147,17 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19">
         <v>0</v>
       </c>
     </row>
@@ -3976,7 +4168,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3997,7 +4189,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4005,7 +4197,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4013,7 +4205,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4021,7 +4213,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4029,7 +4221,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4037,7 +4229,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4045,7 +4237,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4053,7 +4245,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4061,7 +4253,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4069,7 +4261,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4077,7 +4269,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4085,7 +4277,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4093,7 +4285,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4101,7 +4293,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4109,7 +4301,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4117,9 +4309,17 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19">
         <v>0</v>
       </c>
     </row>
@@ -4130,7 +4330,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4151,7 +4351,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4159,7 +4359,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4167,7 +4367,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4175,7 +4375,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4183,7 +4383,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4191,7 +4391,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4199,7 +4399,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4207,7 +4407,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4215,7 +4415,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4223,7 +4423,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4231,7 +4431,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4239,7 +4439,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4247,7 +4447,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4255,7 +4455,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4263,7 +4463,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4271,9 +4471,17 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19">
         <v>0</v>
       </c>
     </row>
@@ -4284,7 +4492,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4305,7 +4513,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4313,7 +4521,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4321,7 +4529,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4329,7 +4537,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4337,7 +4545,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4345,7 +4553,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4353,7 +4561,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4361,7 +4569,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4369,7 +4577,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4377,7 +4585,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4385,7 +4593,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4393,7 +4601,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4401,7 +4609,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4409,7 +4617,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4417,7 +4625,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4425,9 +4633,17 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19">
         <v>0</v>
       </c>
     </row>
@@ -4438,7 +4654,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4459,7 +4675,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4467,7 +4683,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4475,7 +4691,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4483,7 +4699,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4491,7 +4707,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4499,7 +4715,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4507,7 +4723,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4515,7 +4731,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4523,7 +4739,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4531,7 +4747,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4539,7 +4755,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4547,7 +4763,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4555,7 +4771,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4563,7 +4779,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4571,7 +4787,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4579,9 +4795,17 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19">
         <v>0</v>
       </c>
     </row>
@@ -4592,7 +4816,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4613,7 +4837,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4621,7 +4845,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4629,7 +4853,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4637,7 +4861,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4645,7 +4869,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4653,7 +4877,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4661,7 +4885,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4669,7 +4893,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4677,7 +4901,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4685,7 +4909,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4693,7 +4917,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4701,7 +4925,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4709,7 +4933,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4717,7 +4941,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4725,7 +4949,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4733,9 +4957,17 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19">
         <v>0</v>
       </c>
     </row>
@@ -4746,7 +4978,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4767,7 +4999,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4775,7 +5007,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4783,7 +5015,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4791,7 +5023,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4799,7 +5031,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4807,7 +5039,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4815,7 +5047,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4823,7 +5055,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4831,7 +5063,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4839,7 +5071,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4847,7 +5079,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4855,7 +5087,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4863,7 +5095,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4871,7 +5103,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4879,7 +5111,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4887,9 +5119,17 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualiza datasets e assets
</commit_message>
<xml_diff>
--- a/liga_classica/datasets_liga_classica/Pontuacoes_Liga_Classica_Aluna_Completa.xlsx
+++ b/liga_classica/datasets_liga_classica/Pontuacoes_Liga_Classica_Aluna_Completa.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="57">
   <si>
     <t>Rodada 1</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Rodada 38</t>
+  </si>
+  <si>
+    <t>Arran Katoko FC</t>
   </si>
   <si>
     <t>bugredasmissões</t>
@@ -547,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM19"/>
+  <dimension ref="A1:AM20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2811,6 +2814,125 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20" spans="1:39">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+      <c r="AG20">
+        <v>0</v>
+      </c>
+      <c r="AH20">
+        <v>0</v>
+      </c>
+      <c r="AI20">
+        <v>0</v>
+      </c>
+      <c r="AJ20">
+        <v>0</v>
+      </c>
+      <c r="AK20">
+        <v>0</v>
+      </c>
+      <c r="AL20">
+        <v>0</v>
+      </c>
+      <c r="AM20">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2818,7 +2940,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3999,6 +4121,68 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4006,7 +4190,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4027,7 +4211,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4035,7 +4219,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4043,7 +4227,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4051,7 +4235,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4059,7 +4243,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4067,7 +4251,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4075,7 +4259,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4083,7 +4267,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4099,7 +4283,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4107,7 +4291,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4115,7 +4299,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4123,7 +4307,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4131,7 +4315,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4139,7 +4323,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4147,7 +4331,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4155,9 +4339,17 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
         <v>0</v>
       </c>
     </row>
@@ -4168,7 +4360,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4189,7 +4381,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4197,7 +4389,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4205,7 +4397,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4213,7 +4405,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4221,7 +4413,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4229,7 +4421,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4237,7 +4429,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4245,7 +4437,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4261,7 +4453,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4269,7 +4461,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4277,7 +4469,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4285,7 +4477,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4293,7 +4485,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4301,7 +4493,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4309,7 +4501,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4317,9 +4509,17 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
         <v>0</v>
       </c>
     </row>
@@ -4330,7 +4530,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4351,7 +4551,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4359,7 +4559,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4367,7 +4567,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4375,7 +4575,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4383,7 +4583,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4391,7 +4591,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4399,7 +4599,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4407,7 +4607,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4423,7 +4623,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4431,7 +4631,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4439,7 +4639,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4447,7 +4647,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4455,7 +4655,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4463,7 +4663,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4471,7 +4671,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4479,9 +4679,17 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
         <v>0</v>
       </c>
     </row>
@@ -4492,7 +4700,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4513,7 +4721,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4521,7 +4729,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4529,7 +4737,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4537,7 +4745,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4545,7 +4753,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4553,7 +4761,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4561,7 +4769,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4569,7 +4777,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4585,7 +4793,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4593,7 +4801,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4601,7 +4809,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4609,7 +4817,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4617,7 +4825,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4625,7 +4833,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4633,7 +4841,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4641,9 +4849,17 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
         <v>0</v>
       </c>
     </row>
@@ -4654,7 +4870,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4675,7 +4891,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4683,7 +4899,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4691,7 +4907,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4699,7 +4915,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4707,7 +4923,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4715,7 +4931,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4723,7 +4939,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4731,7 +4947,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4747,7 +4963,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4755,7 +4971,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4763,7 +4979,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4771,7 +4987,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4779,7 +4995,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4787,7 +5003,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4795,7 +5011,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4803,9 +5019,17 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
         <v>0</v>
       </c>
     </row>
@@ -4816,7 +5040,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4837,7 +5061,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4845,7 +5069,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4853,7 +5077,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4861,7 +5085,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4869,7 +5093,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4877,7 +5101,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4885,7 +5109,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4893,7 +5117,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4909,7 +5133,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4917,7 +5141,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4925,7 +5149,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4933,7 +5157,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4941,7 +5165,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4949,7 +5173,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4957,7 +5181,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4965,9 +5189,17 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
         <v>0</v>
       </c>
     </row>
@@ -4978,7 +5210,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4999,7 +5231,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5007,7 +5239,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -5015,7 +5247,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5023,7 +5255,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -5031,7 +5263,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -5039,7 +5271,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -5047,7 +5279,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -5055,7 +5287,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -5071,7 +5303,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -5079,7 +5311,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -5087,7 +5319,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -5095,7 +5327,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -5103,7 +5335,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -5111,7 +5343,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -5119,7 +5351,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -5127,9 +5359,17 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualiza copa leon e reorganiza copa
</commit_message>
<xml_diff>
--- a/liga_classica/datasets_liga_classica/Pontuacoes_Liga_Classica_Aluna_Completa.xlsx
+++ b/liga_classica/datasets_liga_classica/Pontuacoes_Liga_Classica_Aluna_Completa.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="58">
   <si>
     <t>Rodada 1</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>GE Bebum</t>
+  </si>
+  <si>
+    <t>GrioTeam</t>
   </si>
   <si>
     <t>Grêmio_Campeão_LA_27</t>
@@ -550,7 +553,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM20"/>
+  <dimension ref="A1:AM21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2933,6 +2936,125 @@
         <v>0</v>
       </c>
     </row>
+    <row r="21" spans="1:39">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <v>0</v>
+      </c>
+      <c r="AG21">
+        <v>0</v>
+      </c>
+      <c r="AH21">
+        <v>0</v>
+      </c>
+      <c r="AI21">
+        <v>0</v>
+      </c>
+      <c r="AJ21">
+        <v>0</v>
+      </c>
+      <c r="AK21">
+        <v>0</v>
+      </c>
+      <c r="AL21">
+        <v>0</v>
+      </c>
+      <c r="AM21">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2940,7 +3062,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4183,6 +4305,68 @@
         <v>0</v>
       </c>
     </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4190,7 +4374,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4211,7 +4395,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4219,7 +4403,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4227,7 +4411,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4235,7 +4419,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4243,7 +4427,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4251,7 +4435,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4259,7 +4443,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4267,7 +4451,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4275,7 +4459,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4283,7 +4467,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4291,7 +4475,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4299,7 +4483,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4307,7 +4491,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4315,7 +4499,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4323,7 +4507,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4331,7 +4515,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4339,7 +4523,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -4347,9 +4531,17 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
         <v>0</v>
       </c>
     </row>
@@ -4360,7 +4552,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4381,7 +4573,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4389,7 +4581,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4397,7 +4589,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4405,7 +4597,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4413,7 +4605,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4421,7 +4613,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4429,7 +4621,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4437,7 +4629,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4445,7 +4637,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4453,7 +4645,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4461,7 +4653,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4469,7 +4661,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4477,7 +4669,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4485,7 +4677,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4493,7 +4685,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4501,7 +4693,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4509,7 +4701,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -4517,9 +4709,17 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
         <v>0</v>
       </c>
     </row>
@@ -4530,7 +4730,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4551,7 +4751,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4559,7 +4759,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4567,7 +4767,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4575,7 +4775,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4583,7 +4783,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4591,7 +4791,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4599,7 +4799,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4607,7 +4807,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4615,7 +4815,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4623,7 +4823,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4631,7 +4831,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4639,7 +4839,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4647,7 +4847,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4655,7 +4855,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4663,7 +4863,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4671,7 +4871,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4679,7 +4879,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -4687,9 +4887,17 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
         <v>0</v>
       </c>
     </row>
@@ -4700,7 +4908,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4721,7 +4929,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4729,7 +4937,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4737,7 +4945,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4745,7 +4953,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4753,7 +4961,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4761,7 +4969,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4769,7 +4977,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4777,7 +4985,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4785,7 +4993,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4793,7 +5001,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4801,7 +5009,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4809,7 +5017,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4817,7 +5025,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4825,7 +5033,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4833,7 +5041,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4841,7 +5049,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4849,7 +5057,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -4857,9 +5065,17 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
         <v>0</v>
       </c>
     </row>
@@ -4870,7 +5086,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4891,7 +5107,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4899,7 +5115,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4907,7 +5123,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4915,7 +5131,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4923,7 +5139,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -4931,7 +5147,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -4939,7 +5155,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4947,7 +5163,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4955,7 +5171,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4963,7 +5179,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4971,7 +5187,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4979,7 +5195,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4987,7 +5203,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4995,7 +5211,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -5003,7 +5219,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -5011,7 +5227,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -5019,7 +5235,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -5027,9 +5243,17 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
         <v>0</v>
       </c>
     </row>
@@ -5040,7 +5264,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5061,7 +5285,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5069,7 +5293,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -5077,7 +5301,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5085,7 +5309,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -5093,7 +5317,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -5101,7 +5325,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -5109,7 +5333,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -5117,7 +5341,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -5125,7 +5349,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -5133,7 +5357,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -5141,7 +5365,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -5149,7 +5373,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -5157,7 +5381,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -5165,7 +5389,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -5173,7 +5397,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -5181,7 +5405,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -5189,7 +5413,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -5197,9 +5421,17 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
         <v>0</v>
       </c>
     </row>
@@ -5210,7 +5442,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5231,7 +5463,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5239,7 +5471,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -5247,7 +5479,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5255,7 +5487,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -5263,7 +5495,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -5271,7 +5503,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -5279,7 +5511,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -5287,7 +5519,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -5295,7 +5527,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -5303,7 +5535,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -5311,7 +5543,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -5319,7 +5551,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -5327,7 +5559,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -5335,7 +5567,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -5343,7 +5575,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -5351,7 +5583,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -5359,7 +5591,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -5367,9 +5599,17 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualiza parciais na Liga Classica Aluna
</commit_message>
<xml_diff>
--- a/liga_classica/datasets_liga_classica/Pontuacoes_Liga_Classica_Aluna_Completa.xlsx
+++ b/liga_classica/datasets_liga_classica/Pontuacoes_Liga_Classica_Aluna_Completa.xlsx
@@ -10,19 +10,19 @@
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
     <sheet name="Turno 2" sheetId="2" r:id="rId2"/>
     <sheet name="Classif Turno 2" sheetId="3" r:id="rId3"/>
-    <sheet name="Mês - Janeiro" sheetId="4" r:id="rId4"/>
-    <sheet name="Mês - Fevereiro" sheetId="5" r:id="rId5"/>
-    <sheet name="Mês - Março" sheetId="6" r:id="rId6"/>
-    <sheet name="Mês - Abril" sheetId="7" r:id="rId7"/>
-    <sheet name="Mês - Maio" sheetId="8" r:id="rId8"/>
-    <sheet name="Mês - Julho" sheetId="9" r:id="rId9"/>
+    <sheet name="Mes - Janeiro" sheetId="4" r:id="rId4"/>
+    <sheet name="Mes - Fevereiro" sheetId="5" r:id="rId5"/>
+    <sheet name="Mes - Marco" sheetId="6" r:id="rId6"/>
+    <sheet name="Mes - Abril" sheetId="7" r:id="rId7"/>
+    <sheet name="Mes - Maio" sheetId="8" r:id="rId8"/>
+    <sheet name="Mes - Julho" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="59">
   <si>
     <t>Rodada 1</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Texas Club 2026</t>
+  </si>
+  <si>
+    <t>Lider_Rodada</t>
   </si>
 </sst>
 </file>
@@ -553,7 +556,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM21"/>
+  <dimension ref="A1:AM22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -680,7 +683,7 @@
         <v>38</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>51.5</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -799,7 +802,7 @@
         <v>39</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>62.76</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -918,7 +921,7 @@
         <v>40</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>38.46</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1037,7 +1040,7 @@
         <v>41</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>58.17</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1156,7 +1159,7 @@
         <v>42</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>83.5</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1275,7 +1278,7 @@
         <v>43</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>45.46</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1394,7 +1397,7 @@
         <v>44</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>63.76</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1513,7 +1516,7 @@
         <v>45</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>44.65</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1632,7 +1635,7 @@
         <v>46</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>53.06</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1751,7 +1754,7 @@
         <v>47</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>53.91</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1870,7 +1873,7 @@
         <v>48</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>39.66</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1989,7 +1992,7 @@
         <v>49</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>44.26</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2108,7 +2111,7 @@
         <v>50</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>54.36</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -2227,7 +2230,7 @@
         <v>51</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>55.96</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2465,7 +2468,7 @@
         <v>53</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>16.4</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -2584,7 +2587,7 @@
         <v>54</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>52.66</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2703,7 +2706,7 @@
         <v>55</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>67.16</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -2822,7 +2825,7 @@
         <v>56</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>40.4</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -2941,7 +2944,7 @@
         <v>57</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>59.86</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -3052,6 +3055,125 @@
         <v>0</v>
       </c>
       <c r="AM21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39">
+      <c r="A22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <v>0</v>
+      </c>
+      <c r="AG22">
+        <v>0</v>
+      </c>
+      <c r="AH22">
+        <v>0</v>
+      </c>
+      <c r="AI22">
+        <v>0</v>
+      </c>
+      <c r="AJ22">
+        <v>0</v>
+      </c>
+      <c r="AK22">
+        <v>0</v>
+      </c>
+      <c r="AL22">
+        <v>0</v>
+      </c>
+      <c r="AM22">
         <v>0</v>
       </c>
     </row>
@@ -3062,7 +3184,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4364,6 +4486,68 @@
         <v>0</v>
       </c>
       <c r="T21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
         <v>0</v>
       </c>
     </row>
@@ -4565,106 +4749,106 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>83.5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>67.16</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>63.76</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>62.76</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>59.86</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>58.17</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>55.96</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>54.36</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>53.91</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>53.06</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>52.66</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>51.5</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>45.46</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4672,52 +4856,52 @@
         <v>45</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>44.65</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>44.26</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>40.4</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>39.66</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>38.46</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>16.4</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B21">
         <v>0</v>

</xml_diff>

<commit_message>
Atualiza resultados parciais da rodada
</commit_message>
<xml_diff>
--- a/liga_classica/datasets_liga_classica/Pontuacoes_Liga_Classica_Aluna_Completa.xlsx
+++ b/liga_classica/datasets_liga_classica/Pontuacoes_Liga_Classica_Aluna_Completa.xlsx
@@ -2468,7 +2468,7 @@
         <v>53</v>
       </c>
       <c r="B17">
-        <v>59.8</v>
+        <v>60.6</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -4832,7 +4832,7 @@
         <v>53</v>
       </c>
       <c r="B12">
-        <v>59.8</v>
+        <v>60.6</v>
       </c>
     </row>
     <row r="13" spans="1:2">

</xml_diff>